<commit_message>
fix: multiple bug fixes
autoname item from lead item
set Photo Quotation link in PO
fix photo quotation download template filters
set po date in sales confirmation
set supplier details header in sales confirmation email excel
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/sales_confirmation/sales_confirmation.xlsx
+++ b/art_collections/art_collections/doctype/sales_confirmation/sales_confirmation.xlsx
@@ -20,23 +20,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Sales Confirmation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buyer : </t>
   </si>
   <si>
     <t xml:space="preserve">ARTYFETES FACTORY
 ZA DE LA MESNILIERE 
-11 RUE DES QUATRE VENTS 14790 VERSON France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NINGBO HYSEAS IMPORT &amp; EXPORT CO.,LTD.
-RM 135, NO. 85 WENJIAO RD, JIANGBEI DISTRICT, NINGBO CITY, ZHEJIANG PROVINCE
-EMAIL:gracewu@hyseas.com
-TEL:86-574-8758 6916  FAX:86-574-8724 7982</t>
+11 RUE DES QUATRE VENTS 
+14790 VERSON
+France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Details</t>
   </si>
   <si>
     <t xml:space="preserve">Your Number Order :</t>
@@ -48,25 +44,18 @@
     <t xml:space="preserve">Our Number Order :</t>
   </si>
   <si>
-    <t xml:space="preserve">P-150672</t>
-  </si>
-  <si>
     <t xml:space="preserve">Delivery Date :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OCT 30,2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -109,52 +98,37 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="14"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Calibri, Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri, Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,12 +139,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -195,19 +163,19 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -234,72 +202,48 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,7 +292,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFD9EAD3"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -375,6 +319,48 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>432000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1159560</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>135000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image2.jpg" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="432000" y="657720"/>
+          <a:ext cx="727560" cy="733680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -382,11 +368,11 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.79"/>
   </cols>
@@ -413,16 +399,14 @@
       <c r="Q1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -430,17 +414,13 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
+      <c r="L2" s="6"/>
+      <c r="O2" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
@@ -451,19 +431,12 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12" t="n">
-        <v>44754</v>
-      </c>
-      <c r="Q3" s="12"/>
+      <c r="O3" s="7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
@@ -474,70 +447,58 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="11" t="s">
+      <c r="O4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="O5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
     </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="3">
     <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="E2:K4"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="B2:C5"/>
+    <mergeCell ref="E2:K5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -546,5 +507,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor: fix column titles in Sales Confirmation Supplier Excel
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/sales_confirmation/sales_confirmation.xlsx
+++ b/art_collections/art_collections/doctype/sales_confirmation/sales_confirmation.xlsx
@@ -128,7 +128,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,18 +139,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBE33D"/>
-        <bgColor rgb="FFFFCC00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF7B59"/>
-        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -202,7 +190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,14 +224,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,66 +236,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF7B59"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FFBBE33D"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -330,9 +250,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1159560</xdr:colOff>
+      <xdr:colOff>1159200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -345,13 +265,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="432000" y="657720"/>
-          <a:ext cx="727560" cy="733680"/>
+          <a:off x="432000" y="658080"/>
+          <a:ext cx="727200" cy="733320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -369,10 +289,10 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.79"/>
   </cols>
@@ -466,24 +386,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-    </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -501,8 +403,8 @@
     <mergeCell ref="E2:K5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>